<commit_message>
Kamisato, może teraz się nie wywali sam przez siebie.
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kot20\Pulpit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{09985B94-0B82-412A-9B76-882ACEC1233E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A55506-72DA-42CD-B96D-EA61279C3DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5B038800-FC48-4D3E-8225-74D4BD1FD21A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5B038800-FC48-4D3E-8225-74D4BD1FD21A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="44">
   <si>
     <t>Data</t>
   </si>
@@ -65,33 +65,12 @@
     <t>Sobota</t>
   </si>
   <si>
-    <t>08:00 - 10:00</t>
-  </si>
-  <si>
     <t>Egzamin/Zaliczenie</t>
   </si>
   <si>
-    <t>Arkusze kalkulacyjne</t>
-  </si>
-  <si>
-    <t>11 sala w informacji i</t>
-  </si>
-  <si>
-    <t>mgr Martyna Duda</t>
-  </si>
-  <si>
     <t>Grupa: WŁ_IZA_inz_1_NS_K2@1</t>
   </si>
   <si>
-    <t>2 termin zaliczenia, na Moodle</t>
-  </si>
-  <si>
-    <t>(tutaj przycisk dołączenia na teams z linkiem)</t>
-  </si>
-  <si>
-    <t>Sobota 10.01.2026</t>
-  </si>
-  <si>
     <t>13:10 - 14:40</t>
   </si>
   <si>
@@ -128,37 +107,67 @@
     <t>Wykład</t>
   </si>
   <si>
-    <t>Finanse</t>
-  </si>
-  <si>
-    <t>03 on-line O</t>
-  </si>
-  <si>
-    <t>dr hab. Magdalena Redo</t>
-  </si>
-  <si>
     <t>Grupa: WŁ_IZA_inz_1_NS_W</t>
   </si>
   <si>
     <t>09:40 - 11:10</t>
   </si>
   <si>
-    <t>04 on-line O</t>
-  </si>
-  <si>
     <t>11:20 - 12:50</t>
   </si>
   <si>
     <t>dr Lidia Mosińska</t>
   </si>
   <si>
-    <t>05 on-line O</t>
-  </si>
-  <si>
     <t>Podstawy rysunku technicznego</t>
   </si>
   <si>
     <t>dr inż. Wojciech Lewandowski</t>
+  </si>
+  <si>
+    <t>Zajęcia w sali A202 Laboratorium automatyki, sala bez zmiana - Zaliczenie I termin</t>
+  </si>
+  <si>
+    <t>Inżynieria materiałowa</t>
+  </si>
+  <si>
+    <t>A304 A</t>
+  </si>
+  <si>
+    <t>mgr inż. Adam Krzywiec</t>
+  </si>
+  <si>
+    <t>02 on-line O</t>
+  </si>
+  <si>
+    <t>A005 A</t>
+  </si>
+  <si>
+    <t>Zaliczenie I termin</t>
+  </si>
+  <si>
+    <t>15 on-line O</t>
+  </si>
+  <si>
+    <t>dr inż. Tomasz Karasiewicz</t>
+  </si>
+  <si>
+    <t>Zarządzanie</t>
+  </si>
+  <si>
+    <t>dr Andrzej Marjański</t>
+  </si>
+  <si>
+    <t>18:20 - 19:50</t>
+  </si>
+  <si>
+    <t>16 on-line O</t>
+  </si>
+  <si>
+    <t>Grupa: WŁ_IZA_inz_1_NS_K1,WŁ_IZA_inz_1_NS_K2</t>
+  </si>
+  <si>
+    <t>Zaliczenie II termin</t>
   </si>
 </sst>
 </file>
@@ -532,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5486A4A7-DD25-42B5-9C07-066EBEC10B8A}">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,39 +580,38 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" t="s">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>46053</v>
+      </c>
+      <c r="F3" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="F3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -611,35 +619,35 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G5" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>46039</v>
+        <v>46053</v>
       </c>
       <c r="F6" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -650,32 +658,29 @@
         <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E8" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="F8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>46039</v>
+        <v>46053</v>
       </c>
       <c r="F9" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F10" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -683,200 +688,368 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E11" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="F11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>46039</v>
+        <v>46053</v>
       </c>
       <c r="F12" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
         <v>27</v>
       </c>
-      <c r="B14" t="s">
+      <c r="E14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" t="s">
         <v>28</v>
-      </c>
-      <c r="C14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" t="s">
-        <v>31</v>
-      </c>
-      <c r="F14" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>46040</v>
+        <v>46054</v>
       </c>
       <c r="F15" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="D17" t="s">
         <v>30</v>
       </c>
       <c r="E17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F17" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>46040</v>
+        <v>46067</v>
       </c>
       <c r="F18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" t="s">
+        <v>32</v>
+      </c>
+      <c r="G20" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>46067</v>
+      </c>
+      <c r="F21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E23" t="s">
         <v>36</v>
-      </c>
-      <c r="C20" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" t="s">
-        <v>20</v>
-      </c>
-      <c r="E20" t="s">
-        <v>31</v>
-      </c>
-      <c r="F20" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>46040</v>
-      </c>
-      <c r="F21" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F22" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" t="s">
-        <v>29</v>
-      </c>
-      <c r="D23" t="s">
-        <v>20</v>
-      </c>
-      <c r="E23" t="s">
-        <v>38</v>
       </c>
       <c r="F23" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>46040</v>
+        <v>46068</v>
       </c>
       <c r="F24" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F25" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B26" t="s">
         <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D26" t="s">
+        <v>27</v>
+      </c>
+      <c r="E26" t="s">
+        <v>36</v>
+      </c>
+      <c r="F26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>46068</v>
+      </c>
+      <c r="F27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" t="s">
+        <v>38</v>
+      </c>
+      <c r="E29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F29" t="s">
         <v>39</v>
       </c>
-      <c r="E26" t="s">
-        <v>31</v>
-      </c>
-      <c r="F26" t="s">
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>46068</v>
+      </c>
+      <c r="F30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" t="s">
+        <v>38</v>
+      </c>
+      <c r="E32" t="s">
+        <v>36</v>
+      </c>
+      <c r="F32" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>46068</v>
+      </c>
+      <c r="F33" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F34" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" t="s">
+        <v>13</v>
+      </c>
+      <c r="E35" t="s">
+        <v>36</v>
+      </c>
+      <c r="F35" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>46068</v>
+      </c>
+      <c r="F36" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>46040</v>
-      </c>
-      <c r="F27" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F28" t="s">
-        <v>31</v>
+      <c r="C38" t="s">
+        <v>22</v>
+      </c>
+      <c r="D38" t="s">
+        <v>13</v>
+      </c>
+      <c r="E38" t="s">
+        <v>36</v>
+      </c>
+      <c r="F38" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>46068</v>
+      </c>
+      <c r="F39" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F40" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41" t="s">
+        <v>21</v>
+      </c>
+      <c r="C41" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" t="s">
+        <v>30</v>
+      </c>
+      <c r="E41" t="s">
+        <v>41</v>
+      </c>
+      <c r="F41" t="s">
+        <v>32</v>
+      </c>
+      <c r="G41" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>46074</v>
+      </c>
+      <c r="F42" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F43" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"Readded schedule and working announcement command"
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kot20\Pulpit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A55506-72DA-42CD-B96D-EA61279C3DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{810BDC0D-3C82-4119-8949-C571D3D1E236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5B038800-FC48-4D3E-8225-74D4BD1FD21A}"/>
+    <workbookView xWindow="6420" yWindow="3450" windowWidth="13470" windowHeight="6390" xr2:uid="{5B038800-FC48-4D3E-8225-74D4BD1FD21A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="65">
   <si>
     <t>Data</t>
   </si>
@@ -168,6 +168,69 @@
   </si>
   <si>
     <t>Zaliczenie II termin</t>
+  </si>
+  <si>
+    <t>Czwartek</t>
+  </si>
+  <si>
+    <t>18:00 - 19:00</t>
+  </si>
+  <si>
+    <t>Inne</t>
+  </si>
+  <si>
+    <t>Spotkanie z menedżerem kierunku</t>
+  </si>
+  <si>
+    <t>19 on-line O</t>
+  </si>
+  <si>
+    <t>dr Piotr Bojar</t>
+  </si>
+  <si>
+    <t>link do zajęć - online</t>
+  </si>
+  <si>
+    <t>04 on-line O</t>
+  </si>
+  <si>
+    <t>05 on-line O</t>
+  </si>
+  <si>
+    <t>Arkusze kalkulacyjne</t>
+  </si>
+  <si>
+    <t>mgr Martyna Duda</t>
+  </si>
+  <si>
+    <t>Finanse</t>
+  </si>
+  <si>
+    <t>08 on-line O</t>
+  </si>
+  <si>
+    <t>dr hab. Magdalena Redo</t>
+  </si>
+  <si>
+    <t>06 on-line O</t>
+  </si>
+  <si>
+    <t>07 on-line O</t>
+  </si>
+  <si>
+    <t>1 termin zaliczenia</t>
+  </si>
+  <si>
+    <t>08:00 - 10:00</t>
+  </si>
+  <si>
+    <t>11 sala w informacji i</t>
+  </si>
+  <si>
+    <t>2 termin zaliczenia, na Moodle</t>
+  </si>
+  <si>
+    <t>03 on-line O</t>
   </si>
 </sst>
 </file>
@@ -541,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5486A4A7-DD25-42B5-9C07-066EBEC10B8A}">
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:H112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71:H114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,38 +643,38 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
+        <v>49</v>
+      </c>
+      <c r="H2" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>46053</v>
+        <v>45995</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -619,35 +682,35 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="H5" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>46053</v>
+        <v>46004</v>
       </c>
       <c r="F6" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -655,32 +718,35 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="F8" t="s">
-        <v>32</v>
+        <v>28</v>
+      </c>
+      <c r="H8" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>46053</v>
+        <v>46004</v>
       </c>
       <c r="F9" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F10" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -688,57 +754,63 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="E11" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="F11" t="s">
-        <v>32</v>
+        <v>54</v>
+      </c>
+      <c r="H11" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>46053</v>
+        <v>46004</v>
       </c>
       <c r="F12" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
         <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="E14" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="F14" t="s">
-        <v>28</v>
+        <v>54</v>
+      </c>
+      <c r="H14" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>46054</v>
+        <v>46004</v>
       </c>
       <c r="F15" t="s">
         <v>10</v>
@@ -746,84 +818,87 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D17" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="E17" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="F17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="H17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>46067</v>
+        <v>46011</v>
       </c>
       <c r="F18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F19" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D20" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="E20" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="F20" t="s">
-        <v>32</v>
-      </c>
-      <c r="G20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="H20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>46067</v>
+        <v>46011</v>
       </c>
       <c r="F21" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F22" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C23" t="s">
         <v>22</v>
@@ -832,64 +907,70 @@
         <v>30</v>
       </c>
       <c r="E23" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="F23" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>46068</v>
+        <v>46011</v>
       </c>
       <c r="F24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F25" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="C26" t="s">
         <v>22</v>
       </c>
       <c r="D26" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E26" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F26" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="H26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>46068</v>
+        <v>46011</v>
       </c>
       <c r="F27" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F28" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C29" t="s">
         <v>22</v>
@@ -898,31 +979,34 @@
         <v>38</v>
       </c>
       <c r="E29" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F29" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>46068</v>
+        <v>46011</v>
       </c>
       <c r="F30" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F31" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C32" t="s">
         <v>22</v>
@@ -931,124 +1015,919 @@
         <v>38</v>
       </c>
       <c r="E32" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="F32" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>46068</v>
+        <v>46011</v>
       </c>
       <c r="F33" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F34" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>20</v>
       </c>
       <c r="B35" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C35" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="D35" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="E35" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="F35" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="G35" t="s">
+        <v>60</v>
+      </c>
+      <c r="H35" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>46068</v>
+        <v>46012</v>
       </c>
       <c r="F36" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F37" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>20</v>
       </c>
       <c r="B38" t="s">
+        <v>25</v>
+      </c>
+      <c r="C38" t="s">
+        <v>12</v>
+      </c>
+      <c r="D38" t="s">
+        <v>27</v>
+      </c>
+      <c r="E38" t="s">
+        <v>52</v>
+      </c>
+      <c r="F38" t="s">
+        <v>28</v>
+      </c>
+      <c r="H38" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>46012</v>
+      </c>
+      <c r="F39" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F40" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>20</v>
+      </c>
+      <c r="B41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" t="s">
+        <v>12</v>
+      </c>
+      <c r="D41" t="s">
+        <v>27</v>
+      </c>
+      <c r="E41" t="s">
+        <v>59</v>
+      </c>
+      <c r="F41" t="s">
+        <v>28</v>
+      </c>
+      <c r="H41" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>46012</v>
+      </c>
+      <c r="F42" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F43" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>8</v>
+      </c>
+      <c r="B44" t="s">
+        <v>61</v>
+      </c>
+      <c r="C44" t="s">
+        <v>9</v>
+      </c>
+      <c r="D44" t="s">
+        <v>53</v>
+      </c>
+      <c r="E44" t="s">
+        <v>62</v>
+      </c>
+      <c r="F44" t="s">
+        <v>54</v>
+      </c>
+      <c r="G44" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>46032</v>
+      </c>
+      <c r="F45" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F46" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>8</v>
+      </c>
+      <c r="B47" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47" t="s">
+        <v>12</v>
+      </c>
+      <c r="D47" t="s">
+        <v>13</v>
+      </c>
+      <c r="E47" t="s">
+        <v>14</v>
+      </c>
+      <c r="F47" t="s">
+        <v>15</v>
+      </c>
+      <c r="G47" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>46039</v>
+      </c>
+      <c r="F48" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F49" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>8</v>
+      </c>
+      <c r="B50" t="s">
+        <v>18</v>
+      </c>
+      <c r="C50" t="s">
+        <v>12</v>
+      </c>
+      <c r="D50" t="s">
+        <v>13</v>
+      </c>
+      <c r="E50" t="s">
+        <v>14</v>
+      </c>
+      <c r="F50" t="s">
+        <v>15</v>
+      </c>
+      <c r="G50" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>46039</v>
+      </c>
+      <c r="F51" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F52" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>8</v>
+      </c>
+      <c r="B53" t="s">
+        <v>19</v>
+      </c>
+      <c r="C53" t="s">
+        <v>12</v>
+      </c>
+      <c r="D53" t="s">
+        <v>13</v>
+      </c>
+      <c r="E53" t="s">
+        <v>14</v>
+      </c>
+      <c r="F53" t="s">
+        <v>15</v>
+      </c>
+      <c r="G53" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>46039</v>
+      </c>
+      <c r="F54" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F55" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>20</v>
+      </c>
+      <c r="B56" t="s">
+        <v>21</v>
+      </c>
+      <c r="C56" t="s">
+        <v>22</v>
+      </c>
+      <c r="D56" t="s">
+        <v>55</v>
+      </c>
+      <c r="E56" t="s">
+        <v>64</v>
+      </c>
+      <c r="F56" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>46040</v>
+      </c>
+      <c r="F57" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F58" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>20</v>
+      </c>
+      <c r="B59" t="s">
+        <v>24</v>
+      </c>
+      <c r="C59" t="s">
+        <v>22</v>
+      </c>
+      <c r="D59" t="s">
+        <v>55</v>
+      </c>
+      <c r="E59" t="s">
+        <v>51</v>
+      </c>
+      <c r="F59" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>46040</v>
+      </c>
+      <c r="F60" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F61" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>20</v>
+      </c>
+      <c r="B62" t="s">
+        <v>25</v>
+      </c>
+      <c r="C62" t="s">
+        <v>22</v>
+      </c>
+      <c r="D62" t="s">
+        <v>13</v>
+      </c>
+      <c r="E62" t="s">
+        <v>64</v>
+      </c>
+      <c r="F62" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>46040</v>
+      </c>
+      <c r="F63" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F64" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>20</v>
+      </c>
+      <c r="B65" t="s">
+        <v>11</v>
+      </c>
+      <c r="C65" t="s">
+        <v>22</v>
+      </c>
+      <c r="D65" t="s">
+        <v>13</v>
+      </c>
+      <c r="E65" t="s">
+        <v>52</v>
+      </c>
+      <c r="F65" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>46040</v>
+      </c>
+      <c r="F66" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F67" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>20</v>
+      </c>
+      <c r="B68" t="s">
+        <v>18</v>
+      </c>
+      <c r="C68" t="s">
+        <v>22</v>
+      </c>
+      <c r="D68" t="s">
+        <v>27</v>
+      </c>
+      <c r="E68" t="s">
+        <v>64</v>
+      </c>
+      <c r="F68" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>46040</v>
+      </c>
+      <c r="F69" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F70" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>8</v>
+      </c>
+      <c r="B71" t="s">
+        <v>21</v>
+      </c>
+      <c r="C71" t="s">
+        <v>12</v>
+      </c>
+      <c r="D71" t="s">
+        <v>13</v>
+      </c>
+      <c r="E71" t="s">
+        <v>14</v>
+      </c>
+      <c r="F71" t="s">
+        <v>15</v>
+      </c>
+      <c r="G71" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>46053</v>
+      </c>
+      <c r="F72" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F73" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>8</v>
+      </c>
+      <c r="B74" t="s">
+        <v>24</v>
+      </c>
+      <c r="C74" t="s">
+        <v>12</v>
+      </c>
+      <c r="D74" t="s">
+        <v>13</v>
+      </c>
+      <c r="E74" t="s">
+        <v>14</v>
+      </c>
+      <c r="F74" t="s">
+        <v>15</v>
+      </c>
+      <c r="G74" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>46053</v>
+      </c>
+      <c r="F75" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F76" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>8</v>
+      </c>
+      <c r="B77" t="s">
+        <v>25</v>
+      </c>
+      <c r="C77" t="s">
+        <v>12</v>
+      </c>
+      <c r="D77" t="s">
+        <v>30</v>
+      </c>
+      <c r="E77" t="s">
+        <v>31</v>
+      </c>
+      <c r="F77" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>46053</v>
+      </c>
+      <c r="F78" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F79" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>8</v>
+      </c>
+      <c r="B80" t="s">
+        <v>11</v>
+      </c>
+      <c r="C80" t="s">
+        <v>12</v>
+      </c>
+      <c r="D80" t="s">
+        <v>30</v>
+      </c>
+      <c r="E80" t="s">
+        <v>31</v>
+      </c>
+      <c r="F80" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>46053</v>
+      </c>
+      <c r="F81" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F82" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>20</v>
+      </c>
+      <c r="B83" t="s">
+        <v>21</v>
+      </c>
+      <c r="C83" t="s">
+        <v>12</v>
+      </c>
+      <c r="D83" t="s">
+        <v>27</v>
+      </c>
+      <c r="E83" t="s">
+        <v>33</v>
+      </c>
+      <c r="F83" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>46054</v>
+      </c>
+      <c r="F84" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F85" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>8</v>
+      </c>
+      <c r="B86" t="s">
+        <v>25</v>
+      </c>
+      <c r="C86" t="s">
+        <v>12</v>
+      </c>
+      <c r="D86" t="s">
+        <v>30</v>
+      </c>
+      <c r="E86" t="s">
+        <v>34</v>
+      </c>
+      <c r="F86" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>46067</v>
+      </c>
+      <c r="F87" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F88" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>8</v>
+      </c>
+      <c r="B89" t="s">
+        <v>11</v>
+      </c>
+      <c r="C89" t="s">
+        <v>12</v>
+      </c>
+      <c r="D89" t="s">
+        <v>30</v>
+      </c>
+      <c r="E89" t="s">
+        <v>34</v>
+      </c>
+      <c r="F89" t="s">
+        <v>32</v>
+      </c>
+      <c r="G89" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>46067</v>
+      </c>
+      <c r="F90" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F91" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>20</v>
+      </c>
+      <c r="B92" t="s">
+        <v>24</v>
+      </c>
+      <c r="C92" t="s">
+        <v>22</v>
+      </c>
+      <c r="D92" t="s">
+        <v>30</v>
+      </c>
+      <c r="E92" t="s">
+        <v>36</v>
+      </c>
+      <c r="F92" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
+        <v>46068</v>
+      </c>
+      <c r="F93" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F94" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>20</v>
+      </c>
+      <c r="B95" t="s">
+        <v>25</v>
+      </c>
+      <c r="C95" t="s">
+        <v>22</v>
+      </c>
+      <c r="D95" t="s">
+        <v>27</v>
+      </c>
+      <c r="E95" t="s">
+        <v>36</v>
+      </c>
+      <c r="F95" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <v>46068</v>
+      </c>
+      <c r="F96" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F97" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>20</v>
+      </c>
+      <c r="B98" t="s">
+        <v>11</v>
+      </c>
+      <c r="C98" t="s">
+        <v>22</v>
+      </c>
+      <c r="D98" t="s">
+        <v>38</v>
+      </c>
+      <c r="E98" t="s">
+        <v>36</v>
+      </c>
+      <c r="F98" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
+        <v>46068</v>
+      </c>
+      <c r="F99" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F100" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>20</v>
+      </c>
+      <c r="B101" t="s">
+        <v>18</v>
+      </c>
+      <c r="C101" t="s">
+        <v>22</v>
+      </c>
+      <c r="D101" t="s">
+        <v>38</v>
+      </c>
+      <c r="E101" t="s">
+        <v>36</v>
+      </c>
+      <c r="F101" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" s="1">
+        <v>46068</v>
+      </c>
+      <c r="F102" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F103" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>20</v>
+      </c>
+      <c r="B104" t="s">
+        <v>19</v>
+      </c>
+      <c r="C104" t="s">
+        <v>22</v>
+      </c>
+      <c r="D104" t="s">
+        <v>13</v>
+      </c>
+      <c r="E104" t="s">
+        <v>36</v>
+      </c>
+      <c r="F104" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" s="1">
+        <v>46068</v>
+      </c>
+      <c r="F105" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F106" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>20</v>
+      </c>
+      <c r="B107" t="s">
         <v>40</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C107" t="s">
         <v>22</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D107" t="s">
         <v>13</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E107" t="s">
         <v>36</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F107" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108" s="1">
         <v>46068</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F108" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F40" t="s">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F109" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
         <v>8</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B110" t="s">
         <v>21</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C110" t="s">
         <v>9</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D110" t="s">
         <v>30</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E110" t="s">
         <v>41</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F110" t="s">
         <v>32</v>
       </c>
-      <c r="G41" t="s">
+      <c r="G110" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111" s="1">
         <v>46074</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F111" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F43" t="s">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F112" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1058,6 +1937,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101004D7BDBFC906D5C418C4E6614C9C8D53B" ma:contentTypeVersion="5" ma:contentTypeDescription="Utwórz nowy dokument." ma:contentTypeScope="" ma:versionID="2206e7bda8c4354471b800aa50dce764">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="716331ec-3935-490f-8606-88c827adc4eb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7831587bcb751c6842357824bbc7163a" ns3:_="">
     <xsd:import namespace="716331ec-3935-490f-8606-88c827adc4eb"/>
@@ -1207,15 +2095,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1225,6 +2104,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{373C0486-46D4-493C-A317-25697048F310}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96BE1156-8FB6-4364-92FE-7F01153CE4F1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1238,14 +2125,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{373C0486-46D4-493C-A317-25697048F310}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>